<commit_message>
Hope this new dictionary thing works well
</commit_message>
<xml_diff>
--- a/writeup/results/parse-lengths-2.xlsx
+++ b/writeup/results/parse-lengths-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="parses" sheetId="2" r:id="rId1"/>
@@ -6389,31 +6389,31 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>11.13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>11.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9</c:v>
+                  <c:v>11.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6951,9 +6951,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -7082,7 +7083,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9212540" cy="5614206"/>
+    <xdr:ext cx="9192381" cy="5614206"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -16653,10 +16654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:CD18"/>
+  <dimension ref="B3:CD25"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16714,7 +16715,7 @@
         <v>4.8</v>
       </c>
       <c r="F5">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="G5">
         <v>3607</v>
@@ -16959,7 +16960,7 @@
         <v>7.7</v>
       </c>
       <c r="F6">
-        <v>1.7</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="7" spans="2:82">
@@ -16976,7 +16977,7 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="8" spans="2:82">
@@ -16993,7 +16994,7 @@
         <v>14.2</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="9" spans="2:82">
@@ -17010,7 +17011,7 @@
         <v>19.7</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>11.13</v>
       </c>
       <c r="G9">
         <v>18</v>
@@ -17153,7 +17154,7 @@
         <v>21.2</v>
       </c>
       <c r="F10">
-        <v>1.8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:82">
@@ -17170,7 +17171,7 @@
         <v>26.9</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>11.3</v>
       </c>
       <c r="G11">
         <v>12406</v>
@@ -17313,7 +17314,7 @@
         <v>31.9</v>
       </c>
       <c r="F12">
-        <v>2.2999999999999998</v>
+        <v>7.9</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -17375,7 +17376,7 @@
         <v>43.3</v>
       </c>
       <c r="F13">
-        <v>1.9</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="14" spans="2:82">
@@ -17466,7 +17467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="7:18">
+    <row r="18" spans="7:21">
       <c r="G18">
         <v>348776</v>
       </c>
@@ -17502,6 +17503,47 @@
       </c>
       <c r="R18">
         <v>326259</v>
+      </c>
+    </row>
+    <row r="25" spans="7:21">
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>8</v>
+      </c>
+      <c r="L25">
+        <v>10</v>
+      </c>
+      <c r="M25">
+        <v>9</v>
+      </c>
+      <c r="N25">
+        <v>8</v>
+      </c>
+      <c r="O25">
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>19</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>3</v>
+      </c>
+      <c r="S25">
+        <v>3</v>
+      </c>
+      <c r="T25">
+        <v>19</v>
+      </c>
+      <c r="U25">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove big files, write words
</commit_message>
<xml_diff>
--- a/writeup/results/parse-lengths-2.xlsx
+++ b/writeup/results/parse-lengths-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="parses" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="canon + constrain" sheetId="7" r:id="rId7"/>
     <sheet name="ConstrainParse" sheetId="9" r:id="rId8"/>
     <sheet name="concat-original-canonical" sheetId="8" r:id="rId9"/>
+    <sheet name="evaluations-with-without-const" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Length</t>
   </si>
@@ -55,12 +56,45 @@
   <si>
     <t>Unconstrained</t>
   </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>With Length Constraints</t>
+  </si>
+  <si>
+    <t>Clue Length</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>57778]</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +143,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,7 +167,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,14 +185,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -161,6 +217,13 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -169,6 +232,13 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4504,11 +4574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073905384"/>
-        <c:axId val="2076606200"/>
+        <c:axId val="2103531304"/>
+        <c:axId val="2094122952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073905384"/>
+        <c:axId val="2103531304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4541,12 +4611,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076606200"/>
+        <c:crossAx val="2094122952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076606200"/>
+        <c:axId val="2094122952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4577,7 +4647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073905384"/>
+        <c:crossAx val="2103531304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4645,7 +4715,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4655,7 +4724,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4665,7 +4733,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="35"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4675,7 +4742,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="36"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4685,7 +4751,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="66"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4695,7 +4760,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="67"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -5164,11 +5228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076694168"/>
-        <c:axId val="2076699720"/>
+        <c:axId val="2104605672"/>
+        <c:axId val="2104611224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076694168"/>
+        <c:axId val="2104605672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -5191,20 +5255,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076699720"/>
+        <c:crossAx val="2104611224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076699720"/>
+        <c:axId val="2104611224"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5228,14 +5291,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076694168"/>
+        <c:crossAx val="2104605672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5262,7 +5324,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5744,11 +5805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076732552"/>
-        <c:axId val="2076735512"/>
+        <c:axId val="2104644024"/>
+        <c:axId val="2104646984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076732552"/>
+        <c:axId val="2104644024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5758,12 +5819,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076735512"/>
+        <c:crossAx val="2104646984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076735512"/>
+        <c:axId val="2104646984"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5775,14 +5836,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076732552"/>
+        <c:crossAx val="2104644024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6077,11 +6137,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2073929464"/>
-        <c:axId val="2073935240"/>
+        <c:axId val="2104694024"/>
+        <c:axId val="2104699800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2073929464"/>
+        <c:axId val="2104694024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6108,14 +6168,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073935240"/>
+        <c:crossAx val="2104699800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6123,7 +6182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073935240"/>
+        <c:axId val="2104699800"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6147,14 +6206,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073929464"/>
+        <c:crossAx val="2104694024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6430,11 +6488,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131376088"/>
-        <c:axId val="2131379320"/>
+        <c:axId val="2104713864"/>
+        <c:axId val="2103544488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131376088"/>
+        <c:axId val="2104713864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6499,7 +6557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131379320"/>
+        <c:crossAx val="2103544488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6507,7 +6565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131379320"/>
+        <c:axId val="2103544488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6552,7 +6610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131376088"/>
+        <c:crossAx val="2104713864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6776,11 +6834,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115452504"/>
-        <c:axId val="2115455528"/>
+        <c:axId val="2104767416"/>
+        <c:axId val="2104773192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115452504"/>
+        <c:axId val="2104767416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6824,7 +6882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115455528"/>
+        <c:crossAx val="2104773192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6832,7 +6890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115455528"/>
+        <c:axId val="2104773192"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6873,7 +6931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115452504"/>
+        <c:crossAx val="2104767416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6951,7 +7009,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="189" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6963,7 +7021,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="189" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7083,7 +7141,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9192381" cy="5614206"/>
+    <xdr:ext cx="9199101" cy="5610847"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7110,7 +7168,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9191885" cy="5610902"/>
+    <xdr:ext cx="9199101" cy="5610847"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -16657,7 +16715,7 @@
   <dimension ref="B3:CD25"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17555,4 +17613,773 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:CB28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:80">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:80">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>115786</v>
+      </c>
+    </row>
+    <row r="5" spans="1:80">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>303297</v>
+      </c>
+      <c r="C5">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:80">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4640610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:80">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:80">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:80">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:80">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:80">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="4">
+        <v>234</v>
+      </c>
+      <c r="H11">
+        <v>295</v>
+      </c>
+      <c r="I11">
+        <v>1193</v>
+      </c>
+      <c r="J11">
+        <v>663</v>
+      </c>
+      <c r="K11">
+        <v>868</v>
+      </c>
+      <c r="L11">
+        <v>192</v>
+      </c>
+      <c r="M11">
+        <v>2122</v>
+      </c>
+      <c r="N11">
+        <v>472</v>
+      </c>
+      <c r="O11">
+        <v>913</v>
+      </c>
+      <c r="P11">
+        <v>1102</v>
+      </c>
+      <c r="Q11">
+        <v>695</v>
+      </c>
+      <c r="R11">
+        <v>261</v>
+      </c>
+      <c r="S11">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:80">
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:80">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>115227</v>
+      </c>
+      <c r="H13">
+        <v>908</v>
+      </c>
+      <c r="I13">
+        <v>31339</v>
+      </c>
+      <c r="J13">
+        <v>2370</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>43164</v>
+      </c>
+      <c r="M13">
+        <v>439</v>
+      </c>
+      <c r="N13">
+        <v>1517</v>
+      </c>
+      <c r="O13">
+        <v>36960</v>
+      </c>
+      <c r="P13">
+        <v>16769</v>
+      </c>
+      <c r="Q13">
+        <v>6534</v>
+      </c>
+      <c r="R13">
+        <v>3234</v>
+      </c>
+      <c r="S13">
+        <v>121518</v>
+      </c>
+      <c r="T13">
+        <v>181972</v>
+      </c>
+      <c r="U13">
+        <v>381</v>
+      </c>
+      <c r="V13">
+        <v>372</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>20501</v>
+      </c>
+      <c r="Y13">
+        <v>271173</v>
+      </c>
+      <c r="Z13">
+        <v>721</v>
+      </c>
+      <c r="AA13">
+        <v>21241</v>
+      </c>
+      <c r="AB13">
+        <v>17040</v>
+      </c>
+      <c r="AC13">
+        <v>28755</v>
+      </c>
+      <c r="AD13">
+        <v>67116</v>
+      </c>
+      <c r="AE13">
+        <v>204</v>
+      </c>
+      <c r="AF13">
+        <v>1258</v>
+      </c>
+      <c r="AG13">
+        <v>415</v>
+      </c>
+      <c r="AH13">
+        <v>182476</v>
+      </c>
+      <c r="AI13">
+        <v>1380</v>
+      </c>
+      <c r="AJ13">
+        <v>89550</v>
+      </c>
+      <c r="AK13">
+        <v>61732</v>
+      </c>
+      <c r="AL13">
+        <v>53228</v>
+      </c>
+      <c r="AM13">
+        <v>1196</v>
+      </c>
+      <c r="AN13">
+        <v>413034</v>
+      </c>
+      <c r="AO13">
+        <v>85646</v>
+      </c>
+      <c r="AP13">
+        <v>69336</v>
+      </c>
+      <c r="AQ13">
+        <v>80782</v>
+      </c>
+      <c r="AR13">
+        <v>310388</v>
+      </c>
+      <c r="AS13">
+        <v>7740</v>
+      </c>
+      <c r="AT13">
+        <v>550923</v>
+      </c>
+      <c r="AU13">
+        <v>995237</v>
+      </c>
+      <c r="AV13">
+        <v>119812</v>
+      </c>
+      <c r="AW13">
+        <v>1008558</v>
+      </c>
+      <c r="AX13">
+        <v>72473</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:80">
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:80">
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="4">
+        <v>194052</v>
+      </c>
+      <c r="H15">
+        <v>48731</v>
+      </c>
+      <c r="I15">
+        <v>63216</v>
+      </c>
+      <c r="J15">
+        <v>145601</v>
+      </c>
+      <c r="K15">
+        <v>72948</v>
+      </c>
+      <c r="L15">
+        <v>354202</v>
+      </c>
+      <c r="M15">
+        <v>36696</v>
+      </c>
+      <c r="N15">
+        <v>340712</v>
+      </c>
+      <c r="O15">
+        <v>2600</v>
+      </c>
+      <c r="P15">
+        <v>63357</v>
+      </c>
+      <c r="Q15">
+        <v>17660</v>
+      </c>
+      <c r="R15">
+        <v>28249</v>
+      </c>
+      <c r="S15">
+        <v>1215927</v>
+      </c>
+      <c r="T15">
+        <v>48167</v>
+      </c>
+      <c r="U15">
+        <v>10907</v>
+      </c>
+      <c r="V15">
+        <v>51151</v>
+      </c>
+      <c r="W15">
+        <v>96321</v>
+      </c>
+      <c r="X15">
+        <v>35766</v>
+      </c>
+      <c r="Y15">
+        <v>13646</v>
+      </c>
+      <c r="Z15">
+        <v>3005056</v>
+      </c>
+      <c r="AA15">
+        <v>311</v>
+      </c>
+      <c r="AB15">
+        <v>60773</v>
+      </c>
+      <c r="AC15">
+        <v>502646</v>
+      </c>
+      <c r="AD15">
+        <v>16282</v>
+      </c>
+      <c r="AE15">
+        <v>95826</v>
+      </c>
+      <c r="AF15">
+        <v>1888052</v>
+      </c>
+      <c r="AG15">
+        <v>1227</v>
+      </c>
+      <c r="AH15">
+        <v>392462</v>
+      </c>
+      <c r="AI15">
+        <v>1302</v>
+      </c>
+      <c r="AJ15">
+        <v>1242124</v>
+      </c>
+      <c r="AK15">
+        <v>62153</v>
+      </c>
+      <c r="AL15">
+        <v>983682</v>
+      </c>
+      <c r="AM15">
+        <v>1356</v>
+      </c>
+      <c r="AN15">
+        <v>323263</v>
+      </c>
+      <c r="AO15">
+        <v>384</v>
+      </c>
+      <c r="AP15">
+        <v>79236</v>
+      </c>
+      <c r="AQ15">
+        <v>962083</v>
+      </c>
+      <c r="AR15">
+        <v>309</v>
+      </c>
+      <c r="AS15">
+        <v>383</v>
+      </c>
+      <c r="AT15">
+        <v>245705</v>
+      </c>
+      <c r="AU15">
+        <v>209879</v>
+      </c>
+      <c r="AV15">
+        <v>74921</v>
+      </c>
+      <c r="AW15">
+        <v>52468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:80">
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>137</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>950</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>27</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>48917</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>88</v>
+      </c>
+      <c r="R16">
+        <v>624</v>
+      </c>
+      <c r="S16">
+        <v>440</v>
+      </c>
+      <c r="T16">
+        <v>99</v>
+      </c>
+      <c r="U16">
+        <v>74578</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>104</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>11610</v>
+      </c>
+      <c r="AB16">
+        <v>359</v>
+      </c>
+      <c r="AC16">
+        <v>3919</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>10033</v>
+      </c>
+      <c r="AF16">
+        <v>40331</v>
+      </c>
+      <c r="AG16">
+        <v>22747</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>94509</v>
+      </c>
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>993</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>3</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>12</v>
+      </c>
+      <c r="AS16">
+        <v>17377</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+      <c r="AU16">
+        <v>19</v>
+      </c>
+      <c r="AV16">
+        <v>30</v>
+      </c>
+      <c r="AW16">
+        <v>10</v>
+      </c>
+      <c r="AX16">
+        <v>0</v>
+      </c>
+      <c r="AY16">
+        <v>954</v>
+      </c>
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16">
+        <v>5747</v>
+      </c>
+      <c r="BC16">
+        <v>0</v>
+      </c>
+      <c r="BD16">
+        <v>524</v>
+      </c>
+      <c r="BE16">
+        <v>183</v>
+      </c>
+      <c r="BF16">
+        <v>43</v>
+      </c>
+      <c r="BG16">
+        <v>12</v>
+      </c>
+      <c r="BH16">
+        <v>374</v>
+      </c>
+      <c r="BI16">
+        <v>0</v>
+      </c>
+      <c r="BJ16">
+        <v>0</v>
+      </c>
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="BL16">
+        <v>528</v>
+      </c>
+      <c r="BM16">
+        <v>0</v>
+      </c>
+      <c r="BN16">
+        <v>5330</v>
+      </c>
+      <c r="BO16">
+        <v>0</v>
+      </c>
+      <c r="BP16">
+        <v>0</v>
+      </c>
+      <c r="BQ16">
+        <v>1357</v>
+      </c>
+      <c r="BR16">
+        <v>0</v>
+      </c>
+      <c r="BS16">
+        <v>1598</v>
+      </c>
+      <c r="BT16">
+        <v>0</v>
+      </c>
+      <c r="BU16">
+        <v>7826</v>
+      </c>
+      <c r="BV16">
+        <v>4</v>
+      </c>
+      <c r="BW16">
+        <v>0</v>
+      </c>
+      <c r="BX16">
+        <v>0</v>
+      </c>
+      <c r="BY16">
+        <v>7</v>
+      </c>
+      <c r="BZ16">
+        <v>0</v>
+      </c>
+      <c r="CA16">
+        <v>0</v>
+      </c>
+      <c r="CB16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:22">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>702</v>
+      </c>
+      <c r="H17">
+        <v>627</v>
+      </c>
+      <c r="I17">
+        <v>59511358</v>
+      </c>
+      <c r="J17">
+        <v>190535</v>
+      </c>
+      <c r="K17">
+        <v>2452229</v>
+      </c>
+      <c r="L17">
+        <v>378512</v>
+      </c>
+      <c r="M17">
+        <v>26973</v>
+      </c>
+      <c r="N17">
+        <v>5401</v>
+      </c>
+      <c r="O17">
+        <v>42085</v>
+      </c>
+      <c r="P17">
+        <v>180692</v>
+      </c>
+      <c r="Q17">
+        <v>1462712</v>
+      </c>
+      <c r="R17">
+        <v>695918</v>
+      </c>
+      <c r="S17">
+        <v>603</v>
+      </c>
+      <c r="T17">
+        <v>20206</v>
+      </c>
+    </row>
+    <row r="18" spans="5:22">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="5:22">
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>207289</v>
+      </c>
+      <c r="H19">
+        <v>955822</v>
+      </c>
+      <c r="I19">
+        <v>1847</v>
+      </c>
+      <c r="J19">
+        <v>89303</v>
+      </c>
+      <c r="K19">
+        <v>27927</v>
+      </c>
+      <c r="L19">
+        <v>91128</v>
+      </c>
+      <c r="M19">
+        <v>16429712</v>
+      </c>
+      <c r="N19">
+        <v>1089574</v>
+      </c>
+      <c r="O19">
+        <v>168769</v>
+      </c>
+      <c r="P19">
+        <v>2386</v>
+      </c>
+      <c r="Q19">
+        <v>106381</v>
+      </c>
+      <c r="R19">
+        <v>794748</v>
+      </c>
+      <c r="S19">
+        <v>2132</v>
+      </c>
+      <c r="T19">
+        <v>1204771</v>
+      </c>
+      <c r="U19">
+        <v>1358913</v>
+      </c>
+      <c r="V19">
+        <v>14062</v>
+      </c>
+    </row>
+    <row r="20" spans="5:22">
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="5:22">
+      <c r="K28" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hopefully a lot of my just done work
</commit_message>
<xml_diff>
--- a/writeup/results/parse-lengths-2.xlsx
+++ b/writeup/results/parse-lengths-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="parses" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,9 @@
     <sheet name="canon + constrain" sheetId="7" r:id="rId7"/>
     <sheet name="ConstrainParse" sheetId="9" r:id="rId8"/>
     <sheet name="concat-original-canonical" sheetId="8" r:id="rId9"/>
-    <sheet name="evaluations-with-without-const" sheetId="10" r:id="rId10"/>
+    <sheet name="prefix-constraints" sheetId="12" r:id="rId10"/>
+    <sheet name="length-constraints" sheetId="11" r:id="rId11"/>
+    <sheet name="evaluations-with-without-const" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Length</t>
   </si>
@@ -55,12 +57,6 @@
   </si>
   <si>
     <t>Unconstrained</t>
-  </si>
-  <si>
-    <t>Before</t>
-  </si>
-  <si>
-    <t>With Length Constraints</t>
   </si>
   <si>
     <t>Clue Length</t>
@@ -91,6 +87,15 @@
   </si>
   <si>
     <t>pref</t>
+  </si>
+  <si>
+    <t>Before Constraints</t>
+  </si>
+  <si>
+    <t>w/ Length Constraints</t>
+  </si>
+  <si>
+    <t>w/ Prefix Constraints</t>
   </si>
 </sst>
 </file>
@@ -6965,6 +6970,594 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'evaluations-with-without-const'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>w/ Prefix Constraints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>221.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2273.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11081.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>690.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>443.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'evaluations-with-without-const'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>w/ Length Constraints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2205.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4762.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16723.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2469.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1336.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2146038520"/>
+        <c:axId val="2098839944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146038520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Clue</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2098839944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2098839944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numer of Solutions Evaluated</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146038520"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'evaluations-with-without-const'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Before Constraints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>736.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115786.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>303297.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.64061E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.409047E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'evaluations-with-without-const'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>w/ Length Constraints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'evaluations-with-without-const'!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2205.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4762.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16723.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2469.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2142393928"/>
+        <c:axId val="2142396344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2142393928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Clue</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142396344"/>
+        <c:crossesAt val="1.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2142396344"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+          <c:min val="70.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numer of Solutions Evaluated</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142393928"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -7025,6 +7618,29 @@
 </file>
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="189" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -7176,6 +7792,60 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="9199101" cy="5610847"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9199101" cy="5610847"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9185661" cy="5610847"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -17626,21 +18296,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CH32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:51">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:51">
@@ -17713,12 +18390,23 @@
         <v>690</v>
       </c>
     </row>
+    <row r="8" spans="1:51">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1336</v>
+      </c>
+      <c r="D8">
+        <v>443</v>
+      </c>
+    </row>
     <row r="11" spans="1:51">
       <c r="E11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" s="4">
         <v>234</v>
@@ -17762,7 +18450,7 @@
     </row>
     <row r="12" spans="1:51">
       <c r="F12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>31</v>
@@ -17806,7 +18494,7 @@
     </row>
     <row r="13" spans="1:51">
       <c r="F13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13">
         <v>31</v>
@@ -17850,10 +18538,10 @@
     </row>
     <row r="14" spans="1:51">
       <c r="E14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14">
         <v>115227</v>
@@ -17988,12 +18676,12 @@
         <v>72473</v>
       </c>
       <c r="AY14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:51">
       <c r="F15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G15">
         <v>1269</v>
@@ -18133,7 +18821,7 @@
     </row>
     <row r="16" spans="1:51">
       <c r="F16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <v>1269</v>
@@ -18222,10 +18910,10 @@
     </row>
     <row r="17" spans="5:86">
       <c r="E17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G17" s="4">
         <v>194052</v>
@@ -18359,7 +19047,7 @@
     </row>
     <row r="18" spans="5:86">
       <c r="F18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>137</v>
@@ -18586,7 +19274,7 @@
     </row>
     <row r="19" spans="5:86">
       <c r="F19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -18831,10 +19519,10 @@
     </row>
     <row r="20" spans="5:86">
       <c r="E20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G20">
         <v>702</v>
@@ -18881,7 +19569,7 @@
     </row>
     <row r="21" spans="5:86">
       <c r="F21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -18994,7 +19682,7 @@
     </row>
     <row r="22" spans="5:86">
       <c r="F22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -19107,10 +19795,10 @@
     </row>
     <row r="23" spans="5:86">
       <c r="E23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G23">
         <v>207289</v>
@@ -19163,7 +19851,7 @@
     </row>
     <row r="24" spans="5:86">
       <c r="F24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -19333,7 +20021,7 @@
     </row>
     <row r="25" spans="5:86">
       <c r="F25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G25">
         <v>0</v>

</xml_diff>